<commit_message>
Adicionado cálculo de desvio padrão Alterado o README.md para inglês
</commit_message>
<xml_diff>
--- a/assets/Dataset_No_Outliers.xlsx
+++ b/assets/Dataset_No_Outliers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,12 +436,12 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>t</t>
+          <t>Di (mm)</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>Xi exp</t>
         </is>
       </c>
     </row>
@@ -450,10 +450,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>3.220916768121119</v>
+        <v>0.01309090777198838</v>
       </c>
     </row>
     <row r="3">
@@ -461,10 +461,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>5.201071428571429</v>
       </c>
       <c r="C3" t="n">
-        <v>3.734052596048377</v>
+        <v>0.02268346734018431</v>
       </c>
     </row>
     <row r="4">
@@ -472,10 +472,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>10.40214285714286</v>
       </c>
       <c r="C4" t="n">
-        <v>3.980773046000128</v>
+        <v>0.03762248338819871</v>
       </c>
     </row>
     <row r="5">
@@ -483,10 +483,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>4</v>
+        <v>15.60321428571429</v>
       </c>
       <c r="C5" t="n">
-        <v>4.444763733093019</v>
+        <v>0.05977083533143</v>
       </c>
     </row>
     <row r="6">
@@ -494,10 +494,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>5</v>
+        <v>20.80428571428572</v>
       </c>
       <c r="C6" t="n">
-        <v>4.746046590086498</v>
+        <v>0.09103112088359989</v>
       </c>
     </row>
     <row r="7">
@@ -505,10 +505,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>6</v>
+        <v>26.00535714285714</v>
       </c>
       <c r="C7" t="n">
-        <v>5.945464316790932</v>
+        <v>0.1330337733836711</v>
       </c>
     </row>
     <row r="8">
@@ -516,10 +516,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>7</v>
+        <v>31.20642857142857</v>
       </c>
       <c r="C8" t="n">
-        <v>5.762933265245647</v>
+        <v>0.1867608082790509</v>
       </c>
     </row>
     <row r="9">
@@ -527,10 +527,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>8</v>
+        <v>36.4075</v>
       </c>
       <c r="C9" t="n">
-        <v>6.420797306053475</v>
+        <v>0.2521854744786399</v>
       </c>
     </row>
     <row r="10">
@@ -538,10 +538,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>9</v>
+        <v>41.60857142857143</v>
       </c>
       <c r="C10" t="n">
-        <v>7.287685360932417</v>
+        <v>0.3280297364691219</v>
       </c>
     </row>
     <row r="11">
@@ -549,10 +549,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>10</v>
+        <v>46.80964285714286</v>
       </c>
       <c r="C11" t="n">
-        <v>8.107584983884172</v>
+        <v>0.4117318800502382</v>
       </c>
     </row>
     <row r="12">
@@ -560,10 +560,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>11</v>
+        <v>52.01071428571429</v>
       </c>
       <c r="C12" t="n">
-        <v>10</v>
+        <v>0.4996712014544753</v>
       </c>
     </row>
     <row r="13">
@@ -571,10 +571,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>12</v>
+        <v>57.21178571428572</v>
       </c>
       <c r="C13" t="n">
-        <v>13.46</v>
+        <v>0.5876265675321952</v>
       </c>
     </row>
     <row r="14">
@@ -582,10 +582,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>13</v>
+        <v>62.41285714285716</v>
       </c>
       <c r="C14" t="n">
-        <v>15.67726833691777</v>
+        <v>0.6713745342684518</v>
       </c>
     </row>
     <row r="15">
@@ -593,10 +593,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>14</v>
+        <v>67.61392857142859</v>
       </c>
       <c r="C15" t="n">
-        <v>17.59201577201154</v>
+        <v>0.7472880111307811</v>
       </c>
     </row>
     <row r="16">
@@ -604,10 +604,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>15</v>
+        <v>72.81500000000001</v>
       </c>
       <c r="C16" t="n">
-        <v>17.92873681133869</v>
+        <v>0.8127962811118726</v>
       </c>
     </row>
     <row r="17">
@@ -615,10 +615,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>16</v>
+        <v>78.01607142857144</v>
       </c>
       <c r="C17" t="n">
-        <v>18.20129963726474</v>
+        <v>0.8666116039870732</v>
       </c>
     </row>
     <row r="18">
@@ -626,10 +626,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>17</v>
+        <v>83.21714285714286</v>
       </c>
       <c r="C18" t="n">
-        <v>18.96451407826908</v>
+        <v>0.9086986318356469</v>
       </c>
     </row>
     <row r="19">
@@ -637,10 +637,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>18</v>
+        <v>88.41821428571428</v>
       </c>
       <c r="C19" t="n">
-        <v>19.11306087416918</v>
+        <v>0.9400331445060129</v>
       </c>
     </row>
     <row r="20">
@@ -648,10 +648,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>19</v>
+        <v>93.61928571428571</v>
       </c>
       <c r="C20" t="n">
-        <v>19.51801975170265</v>
+        <v>0.962242189540759</v>
       </c>
     </row>
     <row r="21">
@@ -659,10 +659,109 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
+        <v>98.82035714285713</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.9772276098567154</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="C21" t="n">
-        <v>20.06417600685225</v>
+      <c r="B22" t="n">
+        <v>104.0214285714286</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.9868534779720193</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>109.2225</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.9927397811900183</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="n">
+        <v>114.4235714285714</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.9961664875199779</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="n">
+        <v>119.6246428571428</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.9980655639659218</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="n">
+        <v>124.8257142857143</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.9990674978428111</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="n">
+        <v>130.0267857142857</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0.9995707277667851</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="n">
+        <v>135.2278571428571</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.9998113436816461</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="n">
+        <v>140.4289285714285</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.9999208684709087</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="n">
+        <v>145.63</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.9999683287581669</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add videos - README
</commit_message>
<xml_diff>
--- a/assets/Dataset_No_Outliers.xlsx
+++ b/assets/Dataset_No_Outliers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,12 +436,12 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Di (mm)</t>
+          <t>X</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Xi exp</t>
+          <t>Y</t>
         </is>
       </c>
     </row>
@@ -453,7 +453,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>0.01309090777198838</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
@@ -461,10 +461,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>5.201071428571429</v>
+        <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>0.02268346734018431</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
@@ -472,10 +472,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>10.40214285714286</v>
+        <v>2</v>
       </c>
       <c r="C4" t="n">
-        <v>0.03762248338819871</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5">
@@ -483,10 +483,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>15.60321428571429</v>
+        <v>3</v>
       </c>
       <c r="C5" t="n">
-        <v>0.05977083533143</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6">
@@ -494,10 +494,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>20.80428571428572</v>
+        <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>0.09103112088359989</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7">
@@ -505,10 +505,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>26.00535714285714</v>
+        <v>5</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1330337733836711</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8">
@@ -516,10 +516,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>31.20642857142857</v>
+        <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>0.1867608082790509</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9">
@@ -527,10 +527,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>36.4075</v>
+        <v>7</v>
       </c>
       <c r="C9" t="n">
-        <v>0.2521854744786399</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10">
@@ -538,10 +538,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>41.60857142857143</v>
+        <v>8</v>
       </c>
       <c r="C10" t="n">
-        <v>0.3280297364691219</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11">
@@ -549,10 +549,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>46.80964285714286</v>
+        <v>9</v>
       </c>
       <c r="C11" t="n">
-        <v>0.4117318800502382</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12">
@@ -560,10 +560,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>52.01071428571429</v>
+        <v>10</v>
       </c>
       <c r="C12" t="n">
-        <v>0.4996712014544753</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13">
@@ -571,10 +571,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>57.21178571428572</v>
+        <v>11</v>
       </c>
       <c r="C13" t="n">
-        <v>0.5876265675321952</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14">
@@ -582,10 +582,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>62.41285714285716</v>
+        <v>12</v>
       </c>
       <c r="C14" t="n">
-        <v>0.6713745342684518</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15">
@@ -593,10 +593,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>67.61392857142859</v>
+        <v>13</v>
       </c>
       <c r="C15" t="n">
-        <v>0.7472880111307811</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16">
@@ -604,10 +604,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>72.81500000000001</v>
+        <v>14</v>
       </c>
       <c r="C16" t="n">
-        <v>0.8127962811118726</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17">
@@ -615,10 +615,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>78.01607142857144</v>
+        <v>15</v>
       </c>
       <c r="C17" t="n">
-        <v>0.8666116039870732</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18">
@@ -626,142 +626,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>83.21714285714286</v>
+        <v>16</v>
       </c>
       <c r="C18" t="n">
-        <v>0.9086986318356469</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" t="n">
-        <v>88.41821428571428</v>
-      </c>
-      <c r="C19" t="n">
-        <v>0.9400331445060129</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" t="n">
-        <v>93.61928571428571</v>
-      </c>
-      <c r="C20" t="n">
-        <v>0.962242189540759</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B21" t="n">
-        <v>98.82035714285713</v>
-      </c>
-      <c r="C21" t="n">
-        <v>0.9772276098567154</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B22" t="n">
-        <v>104.0214285714286</v>
-      </c>
-      <c r="C22" t="n">
-        <v>0.9868534779720193</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="B23" t="n">
-        <v>109.2225</v>
-      </c>
-      <c r="C23" t="n">
-        <v>0.9927397811900183</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="B24" t="n">
-        <v>114.4235714285714</v>
-      </c>
-      <c r="C24" t="n">
-        <v>0.9961664875199779</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="B25" t="n">
-        <v>119.6246428571428</v>
-      </c>
-      <c r="C25" t="n">
-        <v>0.9980655639659218</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="B26" t="n">
-        <v>124.8257142857143</v>
-      </c>
-      <c r="C26" t="n">
-        <v>0.9990674978428111</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="B27" t="n">
-        <v>130.0267857142857</v>
-      </c>
-      <c r="C27" t="n">
-        <v>0.9995707277667851</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="B28" t="n">
-        <v>135.2278571428571</v>
-      </c>
-      <c r="C28" t="n">
-        <v>0.9998113436816461</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="B29" t="n">
-        <v>140.4289285714285</v>
-      </c>
-      <c r="C29" t="n">
-        <v>0.9999208684709087</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="B30" t="n">
-        <v>145.63</v>
-      </c>
-      <c r="C30" t="n">
-        <v>0.9999683287581669</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Interpolation ang Charts Upgrades
</commit_message>
<xml_diff>
--- a/assets/Dataset_No_Outliers.xlsx
+++ b/assets/Dataset_No_Outliers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,7 +450,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.3060928</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -461,10 +461,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>3.748975814634527</v>
+        <v>4.738603388729921</v>
       </c>
       <c r="C3" t="n">
-        <v>0.002668748748748749</v>
+        <v>0.001156177677677678</v>
       </c>
     </row>
     <row r="4">
@@ -472,10 +472,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>8.84292403876468</v>
+        <v>7.339947914712358</v>
       </c>
       <c r="C4" t="n">
-        <v>0.006004684684684685</v>
+        <v>0.001849884284284284</v>
       </c>
     </row>
     <row r="5">
@@ -483,10 +483,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>11.51763743732381</v>
+        <v>11.23519217776038</v>
       </c>
       <c r="C5" t="n">
-        <v>0.008006246246246245</v>
+        <v>0.003006061961961962</v>
       </c>
     </row>
     <row r="6">
@@ -494,10 +494,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>14.12909035999616</v>
+        <v>16.04563476924854</v>
       </c>
       <c r="C6" t="n">
-        <v>0.01000780780780781</v>
+        <v>0.004624710710710711</v>
       </c>
     </row>
     <row r="7">
@@ -505,10 +505,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>17.34897438990156</v>
+        <v>19.54107307980702</v>
       </c>
       <c r="C7" t="n">
-        <v>0.01267655655655656</v>
+        <v>0.006012123923923924</v>
       </c>
     </row>
     <row r="8">
@@ -516,10 +516,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>20.14422891030195</v>
+        <v>23.00569908379239</v>
       </c>
       <c r="C8" t="n">
-        <v>0.01534530530530531</v>
+        <v>0.007630772672672673</v>
       </c>
     </row>
     <row r="9">
@@ -527,10 +527,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>22.95498142723581</v>
+        <v>27.86900011229479</v>
       </c>
       <c r="C9" t="n">
-        <v>0.01868124124124124</v>
+        <v>0.01063683463463463</v>
       </c>
     </row>
     <row r="10">
@@ -538,10 +538,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>24.66685943454284</v>
+        <v>30.79460126660187</v>
       </c>
       <c r="C10" t="n">
-        <v>0.02134998998998999</v>
+        <v>0.01318042552552552</v>
       </c>
     </row>
     <row r="11">
@@ -549,10 +549,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>27.33145166357318</v>
+        <v>34.3398220222001</v>
       </c>
       <c r="C11" t="n">
-        <v>0.02668748748748749</v>
+        <v>0.01780513623623623</v>
       </c>
     </row>
     <row r="12">
@@ -560,10 +560,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>29.11580748908219</v>
+        <v>36.39422832549062</v>
       </c>
       <c r="C12" t="n">
-        <v>0.0313577977977978</v>
+        <v>0.02196737587587588</v>
       </c>
     </row>
     <row r="13">
@@ -571,10 +571,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>30.46862980585554</v>
+        <v>37.79655091322297</v>
       </c>
       <c r="C13" t="n">
-        <v>0.03536092092092092</v>
+        <v>0.02589837997997998</v>
       </c>
     </row>
     <row r="14">
@@ -582,10 +582,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>32.56838458759983</v>
+        <v>39.00197108910267</v>
       </c>
       <c r="C14" t="n">
-        <v>0.04269997997997998</v>
+        <v>0.0312167972972973</v>
       </c>
     </row>
     <row r="15">
@@ -593,10 +593,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>33.58760140164743</v>
+        <v>39.62802055302561</v>
       </c>
       <c r="C15" t="n">
-        <v>0.0467031031031031</v>
+        <v>0.03815386336336336</v>
       </c>
     </row>
     <row r="16">
@@ -604,54 +604,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>34.7600159605728</v>
+        <v>39.66155870212616</v>
       </c>
       <c r="C16" t="n">
-        <v>0.0520406006006006</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" t="n">
-        <v>36.18708994452766</v>
-      </c>
-      <c r="C17" t="n">
-        <v>0.06004684684684684</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="B18" t="n">
-        <v>37.81866017906827</v>
-      </c>
-      <c r="C18" t="n">
-        <v>0.07405777777777778</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" t="n">
-        <v>38.34367614669984</v>
-      </c>
-      <c r="C19" t="n">
-        <v>0.0833983983983984</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" t="n">
-        <v>38.49668467753511</v>
-      </c>
-      <c r="C20" t="n">
-        <v>0.09073745745745745</v>
+        <v>0.042316103003003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the possibility of performing curve adjustments using standard deviations.
</commit_message>
<xml_diff>
--- a/assets/Dataset_No_Outliers.xlsx
+++ b/assets/Dataset_No_Outliers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,12 +436,17 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>y</t>
+          <t>X</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>x</t>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Desvio Padrão</t>
         </is>
       </c>
     </row>
@@ -450,10 +455,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>20.17678</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.001</v>
+        <v>4</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.14</v>
       </c>
     </row>
     <row r="3">
@@ -461,10 +469,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>28.02345962915754</v>
+        <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>0.001107107107107107</v>
+        <v>4.5</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.27</v>
       </c>
     </row>
     <row r="4">
@@ -472,10 +483,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>35.01878230358948</v>
+        <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>0.001214214214214214</v>
+        <v>8</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.055</v>
       </c>
     </row>
     <row r="5">
@@ -483,10 +497,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>46.6602152096022</v>
+        <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>0.001428428428428428</v>
+        <v>7.5</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.195</v>
       </c>
     </row>
     <row r="6">
@@ -494,10 +511,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>55.5107955606899</v>
+        <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>0.001642642642642643</v>
+        <v>11</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.375</v>
       </c>
     </row>
     <row r="7">
@@ -505,10 +525,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>61.98024019950408</v>
+        <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>0.001856856856856857</v>
+        <v>10.5</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.08500000000000001</v>
       </c>
     </row>
     <row r="8">
@@ -516,10 +539,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>68.1160332905129</v>
+        <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>0.002178178178178178</v>
+        <v>14</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.665</v>
       </c>
     </row>
     <row r="9">
@@ -527,10 +553,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>72.95051720227829</v>
+        <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>0.002927927927927928</v>
+        <v>14.5</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.7350000000000001</v>
       </c>
     </row>
     <row r="10">
@@ -538,10 +567,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>77.32409550780011</v>
+        <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>0.003998998998998999</v>
+        <v>15</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.46</v>
       </c>
     </row>
     <row r="11">
@@ -549,10 +581,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>81.49529458742298</v>
+        <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>0.006248248248248248</v>
+        <v>17.5</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.25</v>
       </c>
     </row>
     <row r="12">
@@ -560,10 +595,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>84.34679842432701</v>
+        <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>0.00946146146146146</v>
+        <v>20</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.135</v>
       </c>
     </row>
     <row r="13">
@@ -571,10 +609,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>87.98687185195722</v>
+        <v>12</v>
       </c>
       <c r="C13" t="n">
-        <v>0.01385285285285285</v>
+        <v>22.5</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.29</v>
       </c>
     </row>
     <row r="14">
@@ -582,10 +623,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>91.1771611498895</v>
+        <v>13</v>
       </c>
       <c r="C14" t="n">
-        <v>0.01952952952952953</v>
+        <v>20</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.31</v>
       </c>
     </row>
     <row r="15">
@@ -593,10 +637,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>93.9658807256197</v>
+        <v>14</v>
       </c>
       <c r="C15" t="n">
-        <v>0.02606306306306306</v>
+        <v>21.5</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.495</v>
       </c>
     </row>
     <row r="16">
@@ -604,10 +651,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>96.27911983547557</v>
+        <v>15</v>
       </c>
       <c r="C16" t="n">
-        <v>0.03152552552552552</v>
+        <v>26</v>
+      </c>
+      <c r="D16" t="n">
+        <v>1.05</v>
       </c>
     </row>
     <row r="17">
@@ -615,10 +665,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>98.29402977957339</v>
+        <v>16</v>
       </c>
       <c r="C17" t="n">
-        <v>0.03891591591591591</v>
+        <v>28.5</v>
+      </c>
+      <c r="D17" t="n">
+        <v>1.11</v>
       </c>
     </row>
     <row r="18">
@@ -626,10 +679,13 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>99.59680497669818</v>
+        <v>17</v>
       </c>
       <c r="C18" t="n">
-        <v>0.04373573573573573</v>
+        <v>29</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.39</v>
       </c>
     </row>
     <row r="19">
@@ -637,10 +693,13 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>100.766454419282</v>
+        <v>18</v>
       </c>
       <c r="C19" t="n">
-        <v>0.04984084084084085</v>
+        <v>29.5</v>
+      </c>
+      <c r="D19" t="n">
+        <v>1.435</v>
       </c>
     </row>
     <row r="20">
@@ -648,10 +707,13 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>101.5302631919195</v>
+        <v>19</v>
       </c>
       <c r="C20" t="n">
-        <v>0.05455355355355355</v>
+        <v>30</v>
+      </c>
+      <c r="D20" t="n">
+        <v>1.935</v>
       </c>
     </row>
     <row r="21">
@@ -659,76 +721,13 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>103.2716730743327</v>
+        <v>20</v>
       </c>
       <c r="C21" t="n">
-        <v>0.06205105105105106</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B22" t="n">
-        <v>103.1915241658353</v>
-      </c>
-      <c r="C22" t="n">
-        <v>0.06772772772772773</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="B23" t="n">
-        <v>104.0914312590777</v>
-      </c>
-      <c r="C23" t="n">
-        <v>0.07426126126126126</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="B24" t="n">
-        <v>104.9287780287386</v>
-      </c>
-      <c r="C24" t="n">
-        <v>0.07897397397397397</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="B25" t="n">
-        <v>105.2126866653888</v>
-      </c>
-      <c r="C25" t="n">
-        <v>0.08465065065065065</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="B26" t="n">
-        <v>105.212335836013</v>
-      </c>
-      <c r="C26" t="n">
-        <v>0.08807807807807808</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="B27" t="n">
-        <v>105.5424934239414</v>
-      </c>
-      <c r="C27" t="n">
-        <v>0.09246946946946948</v>
+        <v>31.5</v>
+      </c>
+      <c r="D21" t="n">
+        <v>2.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Confidence Interval to Plots
</commit_message>
<xml_diff>
--- a/assets/Dataset_No_Outliers.xlsx
+++ b/assets/Dataset_No_Outliers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,11 +444,6 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Desvio Padrão</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -460,9 +455,6 @@
       <c r="C2" t="n">
         <v>4</v>
       </c>
-      <c r="D2" t="n">
-        <v>0.14</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -474,9 +466,6 @@
       <c r="C3" t="n">
         <v>4.5</v>
       </c>
-      <c r="D3" t="n">
-        <v>0.27</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -488,9 +477,6 @@
       <c r="C4" t="n">
         <v>8</v>
       </c>
-      <c r="D4" t="n">
-        <v>0.055</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -502,9 +488,6 @@
       <c r="C5" t="n">
         <v>7.5</v>
       </c>
-      <c r="D5" t="n">
-        <v>0.195</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -516,9 +499,6 @@
       <c r="C6" t="n">
         <v>11</v>
       </c>
-      <c r="D6" t="n">
-        <v>0.375</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -530,9 +510,6 @@
       <c r="C7" t="n">
         <v>10.5</v>
       </c>
-      <c r="D7" t="n">
-        <v>0.08500000000000001</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -544,9 +521,6 @@
       <c r="C8" t="n">
         <v>14</v>
       </c>
-      <c r="D8" t="n">
-        <v>0.665</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -558,9 +532,6 @@
       <c r="C9" t="n">
         <v>14.5</v>
       </c>
-      <c r="D9" t="n">
-        <v>0.7350000000000001</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -572,9 +543,6 @@
       <c r="C10" t="n">
         <v>15</v>
       </c>
-      <c r="D10" t="n">
-        <v>0.46</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -586,9 +554,6 @@
       <c r="C11" t="n">
         <v>17.5</v>
       </c>
-      <c r="D11" t="n">
-        <v>0.25</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -600,9 +565,6 @@
       <c r="C12" t="n">
         <v>20</v>
       </c>
-      <c r="D12" t="n">
-        <v>0.135</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -614,9 +576,6 @@
       <c r="C13" t="n">
         <v>22.5</v>
       </c>
-      <c r="D13" t="n">
-        <v>0.29</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -628,9 +587,6 @@
       <c r="C14" t="n">
         <v>20</v>
       </c>
-      <c r="D14" t="n">
-        <v>0.31</v>
-      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -642,9 +598,6 @@
       <c r="C15" t="n">
         <v>21.5</v>
       </c>
-      <c r="D15" t="n">
-        <v>0.495</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -656,9 +609,6 @@
       <c r="C16" t="n">
         <v>26</v>
       </c>
-      <c r="D16" t="n">
-        <v>1.05</v>
-      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -670,9 +620,6 @@
       <c r="C17" t="n">
         <v>28.5</v>
       </c>
-      <c r="D17" t="n">
-        <v>1.11</v>
-      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -684,9 +631,6 @@
       <c r="C18" t="n">
         <v>29</v>
       </c>
-      <c r="D18" t="n">
-        <v>0.39</v>
-      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -698,9 +642,6 @@
       <c r="C19" t="n">
         <v>29.5</v>
       </c>
-      <c r="D19" t="n">
-        <v>1.435</v>
-      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -712,9 +653,6 @@
       <c r="C20" t="n">
         <v>30</v>
       </c>
-      <c r="D20" t="n">
-        <v>1.935</v>
-      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -725,9 +663,6 @@
       </c>
       <c r="C21" t="n">
         <v>31.5</v>
-      </c>
-      <c r="D21" t="n">
-        <v>2.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>